<commit_message>
weitere Ergänzungen zum Code....Constraints fehlen noch! Energiesystem2 ist das Aktuelle!
</commit_message>
<xml_diff>
--- a/Legende_Variablen.xlsx
+++ b/Legende_Variablen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ext\OneDrive\Documentos\ModE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C70095D-3BF4-42CE-909E-723CED1F33F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532D0543-C932-4F4A-9F65-336FD1E40996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{D7E2CD79-FCD3-47CC-86ED-0EBA5174B92D}"/>
+    <workbookView xWindow="9105" yWindow="-15870" windowWidth="25440" windowHeight="15990" xr2:uid="{D7E2CD79-FCD3-47CC-86ED-0EBA5174B92D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -209,75 +209,31 @@
     <t>kWh_CH4</t>
   </si>
   <si>
-    <t>FRAGEN</t>
-  </si>
-  <si>
-    <t>Outputs drinnen lassen?</t>
-  </si>
-  <si>
-    <t>declare time dependent parameter, timesliceweight, ect ----Was ist das?</t>
-  </si>
-  <si>
     <t>Constraints</t>
   </si>
   <si>
     <t>decision_variables (für jeden Komponente?, fürs ein und ausspeichern?)</t>
   </si>
   <si>
-    <t>Welchen CarbonPrice?</t>
-  </si>
-  <si>
-    <t>powerpoint: p28 (CarbonPriceExpectations, EU, 2022-2025): 84.4€/ton</t>
-  </si>
-  <si>
-    <t>p15 (Netherlands, 2024) 71.48 $/ton [DE gibt’s nicht]</t>
-  </si>
-  <si>
-    <t>Welcher GasPreis?</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> Commercial, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Industrial</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (2023)</t>
-    </r>
-  </si>
-  <si>
-    <t>Welcher Strompreis?</t>
-  </si>
-  <si>
-    <t>statista</t>
-  </si>
-  <si>
-    <t>24.46 ct€/kWh (2023, industrial customers), vglw. Hoch</t>
-  </si>
-  <si>
-    <t>Jahr 2023, stündlicher Datensatz beiinhaltet negative Werte…zu null?</t>
-  </si>
-  <si>
-    <t>time_slice weight??</t>
-  </si>
-  <si>
     <t>Noch zu tun:</t>
+  </si>
+  <si>
+    <t>y_PEM</t>
+  </si>
+  <si>
+    <t>y_CHP</t>
+  </si>
+  <si>
+    <t>y_BO</t>
+  </si>
+  <si>
+    <t>Elektrolyse (an/aus)</t>
+  </si>
+  <si>
+    <t>Blockheizkraftwerk (an/aus)</t>
+  </si>
+  <si>
+    <t>Boiler (an/aus)</t>
   </si>
 </sst>
 </file>
@@ -301,12 +257,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -321,9 +283,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -658,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59FC6673-EC86-49A3-A2F2-72A45687943D}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -681,28 +644,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -710,308 +662,297 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" s="2" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>36</v>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" t="s">
         <v>40</v>
-      </c>
-      <c r="C20" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" t="s">
         <v>40</v>
       </c>
-      <c r="C22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" t="s">
-        <v>49</v>
+      <c r="A24" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
         <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
         <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A51" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>62</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C38" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>65</v>
-      </c>
-      <c r="B39" t="s">
-        <v>66</v>
-      </c>
-      <c r="C39" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B41" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A45" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>